<commit_message>
Mise à jour du sprint 3
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Sprint.xlsx
+++ b/Documents/Scrum/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CF7C2A-64D8-4068-B8D0-148286C4A766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37AE642-90C7-4E29-8FCC-56563210569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="3610" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_1." sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <t>STORY</t>
   </si>
@@ -105,19 +105,7 @@
     <t>X</t>
   </si>
   <si>
-    <t>Prototype fonctionnel</t>
-  </si>
-  <si>
-    <t>Environnement de test</t>
-  </si>
-  <si>
     <t>Jeux de tests de l'application</t>
-  </si>
-  <si>
-    <t>Document manuel utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document manuel installation </t>
   </si>
   <si>
     <t>Analyser la situation actuelle pour la recherche des lieux</t>
@@ -173,13 +161,65 @@
     <t>Document plan d'assurance qualité</t>
   </si>
   <si>
-    <t>Faire la modélisation de la base de donnée</t>
-  </si>
-  <si>
-    <t>Créer le login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corriger la maquette </t>
+    <t>Maquette</t>
+  </si>
+  <si>
+    <t>Définir commennt on travaille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Écrire ce que l'on va faire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Décrire qui assure la communication 
+entre le groupe d'encadrment et le mandant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Répondre à la question 
+de quoi faire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Répondre à la question 
+de comment le faire </t>
+  </si>
+  <si>
+    <t>Modélisation de la base de donnée</t>
+  </si>
+  <si>
+    <t>Créer la modélisation de la base de donnée</t>
+  </si>
+  <si>
+    <t>Faire les différents jeux de test pour le login</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Création d'accès pour les différents utilisateur</t>
+  </si>
+  <si>
+    <t>Recherche sécurité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire des recherches sur la signature électronique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche sur le privacy by design </t>
+  </si>
+  <si>
+    <t>Rechercher comment créer une API</t>
+  </si>
+  <si>
+    <t>Recherche sur l'API Google Map, agenda</t>
+  </si>
+  <si>
+    <t>Faire la maquette sur l'application Visual Studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document de vision </t>
+  </si>
+  <si>
+    <t>Mettre à jour le document de vision après
+retour du groupe d'encadrement</t>
   </si>
 </sst>
 </file>
@@ -249,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -510,11 +550,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -556,9 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,7 +654,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +1006,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,28 +1016,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
-        <v>31</v>
+      <c r="A2" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -968,9 +1047,9 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -980,9 +1059,9 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -992,9 +1071,9 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1004,9 +1083,9 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1016,9 +1095,9 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1028,9 +1107,9 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1040,11 +1119,11 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
-        <v>38</v>
+      <c r="A9" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1053,9 +1132,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1064,9 +1143,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="30"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1076,9 +1155,9 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="30"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1087,9 +1166,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="30"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1098,9 +1177,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1158,7 +1237,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1172,7 +1251,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="33"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1263,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
@@ -1195,7 +1274,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="33"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1206,7 +1285,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="33"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
@@ -1218,7 +1297,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="33"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1229,7 +1308,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="33"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
@@ -1240,7 +1319,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="33"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="17" t="s">
         <v>14</v>
       </c>
@@ -1251,7 +1330,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1262,7 +1341,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1352,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -1284,7 +1363,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="34"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="17" t="s">
         <v>16</v>
       </c>
@@ -1327,15 +1406,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B15C13B-4F2C-4FF3-B337-5CE0DE76848B}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1357,185 +1437,210 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="36"/>
+      <c r="B4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="4"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="36"/>
+      <c r="B5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="4"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="37"/>
+      <c r="B6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="4"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4"/>
-      <c r="H9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>18</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A11:A14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1736,19 +1841,19 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Création du sprint 4
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Sprint.xlsx
+++ b/Documents/Scrum/Sprint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37AE642-90C7-4E29-8FCC-56563210569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D426CFFE-2D3A-43DE-8980-4E57AB9D4939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_1." sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
   <si>
     <t>STORY</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Document plan d'assurance qualité</t>
   </si>
   <si>
-    <t>Maquette</t>
-  </si>
-  <si>
     <t>Définir commennt on travaille</t>
   </si>
   <si>
@@ -212,21 +209,338 @@
     <t>Recherche sur l'API Google Map, agenda</t>
   </si>
   <si>
-    <t>Faire la maquette sur l'application Visual Studio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Document de vision </t>
   </si>
   <si>
     <t>Mettre à jour le document de vision après
 retour du groupe d'encadrement</t>
+  </si>
+  <si>
+    <t>Maquette (sur Visual Studio)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Créer la view du login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Créer la view du mot de passe oublié</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Créer la view des paramètres </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Créer la view des projets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Créer la view pour le chat </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Créer la view de la page principale</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la page principale</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la view pour les projets </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Créer la view pour la gestion de stock </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Créer la view pour la gestion de projet  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la view pour le chat </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Maquette sur Visual Studio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du login </t>
+  </si>
+  <si>
+    <t>Créer de la base de donnée sur One.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +564,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +626,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -567,7 +923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -627,6 +983,18 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -654,9 +1022,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -666,12 +1031,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -681,7 +1040,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1003,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3F248E-F3B8-4FD5-B554-6BF12D242858}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1033,7 +1449,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1047,7 +1463,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1059,7 +1475,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="26"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1071,7 +1487,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="26"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1083,7 +1499,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1095,7 +1511,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="26"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1107,7 +1523,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1119,22 +1535,19 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1143,32 +1556,32 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="29"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="18" t="s">
         <v>18</v>
       </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="29"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1177,9 +1590,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="30"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1187,17 +1600,28 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="34"/>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A10:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1237,7 +1661,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1251,7 +1675,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="32"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1687,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
@@ -1274,7 +1698,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="32"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1709,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="32"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1721,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="32"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1308,7 +1732,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="32"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
@@ -1319,7 +1743,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="32"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="17" t="s">
         <v>14</v>
       </c>
@@ -1330,7 +1754,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1341,7 +1765,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
@@ -1352,7 +1776,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="32"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -1363,7 +1787,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="17" t="s">
         <v>16</v>
       </c>
@@ -1406,10 +1830,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B15C13B-4F2C-4FF3-B337-5CE0DE76848B}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1419,7 +1843,7 @@
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1436,208 +1860,233 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="38" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="39"/>
+      <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="39"/>
+      <c r="B4" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
-      <c r="B4" s="34" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="39"/>
+      <c r="B5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="36"/>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="40"/>
+      <c r="B6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="37"/>
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="56"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
+      <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="61"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="62"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="39" t="s">
-        <v>19</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="26" t="s">
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>18</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C10" s="28"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="40" t="s">
+      <c r="E10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="61"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="63"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="62"/>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="41"/>
-      <c r="B12" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
-      <c r="B13" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
-      <c r="B14" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
-        <v>53</v>
-      </c>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="42"/>
       <c r="B15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="42"/>
+      <c r="B16" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="43"/>
+      <c r="B17" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="64"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="62"/>
+    </row>
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A14:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1647,18 +2096,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79544C66-D72C-4E56-AF4D-5568E5F5A64B}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1675,158 +2126,285 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="51"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
+      <c r="E4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="46"/>
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
+      <c r="E5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="46"/>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
+      <c r="E6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="46"/>
+      <c r="B7" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
+      <c r="E7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="46"/>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
+      <c r="E8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="46"/>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
+      <c r="E9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="46"/>
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2"/>
+      <c r="E10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="46"/>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2"/>
+      <c r="E11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="46"/>
+      <c r="B12" s="44" t="s">
+        <v>57</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
+      <c r="E12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="46"/>
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
+      <c r="E13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="47"/>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="E14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="52"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="42"/>
+      <c r="B17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>18</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="42"/>
+      <c r="B18" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>18</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="43"/>
+      <c r="B19" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>18</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="53"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="51"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A4:A14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Mise à jour sprint (partie tests)
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Sprint.xlsx
+++ b/Documents/Scrum/Sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D426CFFE-2D3A-43DE-8980-4E57AB9D4939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E017086-D223-4B4C-BF98-4F1B6B94EE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
   <si>
     <t>STORY</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>Créer la modélisation de la base de donnée</t>
-  </si>
-  <si>
-    <t>Faire les différents jeux de test pour le login</t>
   </si>
   <si>
     <t>Login</t>
@@ -354,40 +351,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> : Créer la view de la page principale</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Membre</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Créer la page principale</t>
     </r>
   </si>
   <si>
@@ -534,6 +497,49 @@
   </si>
   <si>
     <t>Créer de la base de donnée sur One.com</t>
+  </si>
+  <si>
+    <t>Créer le test LoginGood()</t>
+  </si>
+  <si>
+    <t>Créer le test LoginWrongPassword()</t>
+  </si>
+  <si>
+    <t>Créer le test LoginWrongEmail()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la view page principale</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -923,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -995,61 +1001,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1099,6 +1054,63 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1449,7 +1461,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="51" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1463,7 +1475,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
+      <c r="A3" s="52"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1475,7 +1487,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1487,7 +1499,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="30"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +1511,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="30"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1511,7 +1523,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="30"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1523,7 +1535,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1535,15 +1547,15 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="54" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1556,7 +1568,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1567,7 +1579,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1579,7 +1591,7 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1602,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
@@ -1601,7 +1613,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="34"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
@@ -1632,7 +1644,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1661,7 +1673,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="57" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1675,7 +1687,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1687,7 +1699,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
@@ -1698,7 +1710,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="36"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1709,7 +1721,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="36"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
@@ -1721,7 +1733,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="36"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1732,7 +1744,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="36"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
@@ -1743,7 +1755,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="36"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="17" t="s">
         <v>14</v>
       </c>
@@ -1754,7 +1766,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1765,7 +1777,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="36"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
@@ -1776,7 +1788,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="36"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -1787,7 +1799,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>16</v>
       </c>
@@ -1832,8 +1844,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1861,7 +1873,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="60" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1875,7 +1887,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
+      <c r="A3" s="61"/>
       <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
@@ -1887,7 +1899,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="25" t="s">
         <v>38</v>
       </c>
@@ -1899,7 +1911,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="17" t="s">
         <v>39</v>
       </c>
@@ -1911,7 +1923,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="17" t="s">
         <v>40</v>
       </c>
@@ -1923,11 +1935,11 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="56"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="60"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1945,19 +1957,19 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="61"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="62"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="2"/>
@@ -1967,40 +1979,40 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="61"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="38" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="63"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="62"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>18</v>
@@ -2009,9 +2021,9 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="42"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>18</v>
@@ -2020,9 +2032,9 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="42"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>18</v>
@@ -2031,9 +2043,9 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="43"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>18</v>
@@ -2042,18 +2054,18 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="64"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="62"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>52</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="2"/>
@@ -2096,10 +2108,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79544C66-D72C-4E56-AF4D-5568E5F5A64B}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2131,54 +2143,46 @@
         <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="69" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="51"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="18" t="s">
-        <v>18</v>
-      </c>
+      <c r="A4" s="30"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="18" t="s">
-        <v>18</v>
-      </c>
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="46"/>
+      <c r="A6" s="66" t="s">
+        <v>52</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="18" t="s">
         <v>18</v>
@@ -2186,7 +2190,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="46"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="2" t="s">
         <v>61</v>
       </c>
@@ -2198,7 +2202,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="46"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="2" t="s">
         <v>60</v>
       </c>
@@ -2210,9 +2214,9 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2222,9 +2226,9 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="46"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2234,9 +2238,9 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="46"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2246,9 +2250,9 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="46"/>
-      <c r="B12" s="44" t="s">
-        <v>57</v>
+      <c r="A12" s="67"/>
+      <c r="B12" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2258,9 +2262,9 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="46"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2270,9 +2274,9 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="47"/>
-      <c r="B14" s="2" t="s">
-        <v>59</v>
+      <c r="A14" s="67"/>
+      <c r="B14" s="29" t="s">
+        <v>56</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2282,53 +2286,54 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="52"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="51"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="68"/>
+      <c r="B16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="35"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="42"/>
-      <c r="B17" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="42"/>
-      <c r="B18" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
-      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="43"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>18</v>
@@ -2337,18 +2342,21 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="51"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>43</v>
+      <c r="A21" s="65"/>
+      <c r="B21" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>18</v>
@@ -2357,39 +2365,53 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="4"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="28"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="38" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="E24" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="68"/>
+      <c r="B25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
@@ -2398,10 +2420,18 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A4:A14"/>
+  <mergeCells count="3">
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A6:A16"/>
+    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Mise à jour sprint 4
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Sprint.xlsx
+++ b/Documents/Scrum/Sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E017086-D223-4B4C-BF98-4F1B6B94EE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BD7F39-E57B-4DB1-BECA-56CC53FD819D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="93">
   <si>
     <t>STORY</t>
   </si>
@@ -496,9 +496,6 @@
     <t xml:space="preserve">Création du login </t>
   </si>
   <si>
-    <t>Créer de la base de donnée sur One.com</t>
-  </si>
-  <si>
     <t>Créer le test LoginGood()</t>
   </si>
   <si>
@@ -540,6 +537,79 @@
       </rPr>
       <t xml:space="preserve"> Créer la view page principale</t>
     </r>
+  </si>
+  <si>
+    <t>Créer la classe Client</t>
+  </si>
+  <si>
+    <t>Créer la classe Personne</t>
+  </si>
+  <si>
+    <t>Créer la classe Photographe</t>
+  </si>
+  <si>
+    <t>Créer la classe Collaborateur</t>
+  </si>
+  <si>
+    <t>Créer la classe Gère</t>
+  </si>
+  <si>
+    <t>Créer la classe Content</t>
+  </si>
+  <si>
+    <t>Créer la classe Évènement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la classe Facture </t>
+  </si>
+  <si>
+    <t>Créer la classe Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la classe Devis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la classe Contrat </t>
+  </si>
+  <si>
+    <t>Créer la classe Projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la classe Concerne </t>
+  </si>
+  <si>
+    <t>Créer la classe Lieu</t>
+  </si>
+  <si>
+    <t>Créer la classe Photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demander les identifianst à Waview  </t>
+  </si>
+  <si>
+    <t>Se connecte et aller sur le serveur + Php my admin</t>
+  </si>
+  <si>
+    <t>Créer la classe Correspond</t>
+  </si>
+  <si>
+    <t>Créer la classe Critère</t>
+  </si>
+  <si>
+    <t>Créer la classe FichierVidéo</t>
+  </si>
+  <si>
+    <t>Créer le classe Consulte</t>
+  </si>
+  <si>
+    <t>Créer la classe A_Lieu</t>
+  </si>
+  <si>
+    <t>Créer la classe Date</t>
+  </si>
+  <si>
+    <t>Créer la base de données 
+sur One.com</t>
   </si>
 </sst>
 </file>
@@ -651,7 +721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -925,11 +995,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1002,9 +1083,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1109,7 +1187,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1461,7 +1553,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1475,7 +1567,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="52"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1487,7 +1579,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="52"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1499,7 +1591,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="52"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1511,7 +1603,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="52"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1523,7 +1615,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="52"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1535,7 +1627,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1547,15 +1639,15 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="48"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="53" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1568,7 +1660,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1579,7 +1671,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1591,7 +1683,7 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
@@ -1602,7 +1694,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
@@ -1613,7 +1705,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
@@ -1644,7 +1736,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1673,7 +1765,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1687,7 +1779,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="58"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1791,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="58"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
@@ -1710,7 +1802,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="58"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1721,7 +1813,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="58"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
@@ -1733,7 +1825,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="58"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1744,7 +1836,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="58"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
@@ -1755,7 +1847,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="58"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="17" t="s">
         <v>14</v>
       </c>
@@ -1766,7 +1858,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="58"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1777,7 +1869,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="58"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
@@ -1788,7 +1880,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="58"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -1799,7 +1891,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="59"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="17" t="s">
         <v>16</v>
       </c>
@@ -1844,7 +1936,7 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1873,7 +1965,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="59" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1887,7 +1979,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="61"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
@@ -1899,7 +1991,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="61"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="25" t="s">
         <v>38</v>
       </c>
@@ -1911,7 +2003,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="61"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="17" t="s">
         <v>39</v>
       </c>
@@ -1923,7 +2015,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="62"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="17" t="s">
         <v>40</v>
       </c>
@@ -1935,11 +2027,11 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="39"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1957,11 +2049,11 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="44"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="45"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1979,11 +2071,11 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="44"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1995,20 +2087,20 @@
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="37" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="46"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="45"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="44"/>
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="62" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -2021,7 +2113,7 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="64"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="17" t="s">
         <v>47</v>
       </c>
@@ -2032,7 +2124,7 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="64"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
@@ -2043,7 +2135,7 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="65"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="17" t="s">
         <v>49</v>
       </c>
@@ -2054,11 +2146,11 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="47"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="45"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
@@ -2108,10 +2200,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79544C66-D72C-4E56-AF4D-5568E5F5A64B}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2139,299 +2231,541 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="54"/>
+      <c r="B3" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="54"/>
+      <c r="B4" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="54"/>
+      <c r="B5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="54"/>
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="54"/>
+      <c r="B7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="69"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="54"/>
+      <c r="B8" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="69"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="54"/>
+      <c r="B9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="54"/>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="54"/>
+      <c r="B11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="54"/>
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="69"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="54"/>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="69"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="54"/>
+      <c r="B14" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="54"/>
+      <c r="B15" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="69"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="54"/>
+      <c r="B16" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="69"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="54"/>
+      <c r="B17" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="69"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="54"/>
+      <c r="B18" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="69"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="54"/>
+      <c r="B19" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="54"/>
+      <c r="B20" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="54"/>
+      <c r="B21" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="54"/>
+      <c r="B22" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="69"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="54"/>
+      <c r="B23" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="55"/>
+      <c r="B24" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="30"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="66"/>
+      <c r="B27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="66"/>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="66"/>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="66"/>
+      <c r="B30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="66"/>
+      <c r="B31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="66"/>
+      <c r="B32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="66"/>
+      <c r="B33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="66"/>
+      <c r="B34" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="66"/>
+      <c r="B35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="67"/>
+      <c r="B36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="34"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="63"/>
+      <c r="B39" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="63"/>
+      <c r="B40" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="4"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="64"/>
+      <c r="B41" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="35"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="33"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="67"/>
-      <c r="B7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="67"/>
-      <c r="B8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="67"/>
-      <c r="B9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="67"/>
-      <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="67"/>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="67"/>
-      <c r="B12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="67"/>
-      <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="67"/>
-      <c r="B14" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="67"/>
-      <c r="B15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="68"/>
-      <c r="B16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="64"/>
-      <c r="B19" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="64"/>
-      <c r="B20" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="65"/>
-      <c r="B21" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="36"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="34"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="C43" s="28"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="66"/>
+      <c r="B44" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="67"/>
-      <c r="B24" s="2" t="s">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="73"/>
+      <c r="B45" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="68"/>
-      <c r="B25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="74" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A6:A16"/>
-    <mergeCell ref="A23:A25"/>
+  <mergeCells count="4">
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A2:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Mise à jour sprint
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Sprint.xlsx
+++ b/Documents/Scrum/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0520BB72-6F8C-47DA-948A-28959F5BB374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA06F5B2-2C01-4722-92C8-E5C3653668D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_0." sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="98">
   <si>
     <t>STORY</t>
   </si>
@@ -624,6 +624,9 @@
   <si>
     <t xml:space="preserve">Lier le calendrier des disponibilités 
 Waview avec leurs calendriers </t>
+  </si>
+  <si>
+    <t>Connecter à la base de données</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1103,20 +1106,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1167,6 +1161,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1212,41 +1224,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1597,7 +1597,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="59" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1611,7 +1611,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="57"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1623,7 +1623,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="57"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="57"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1647,7 +1647,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="57"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="57"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1671,7 +1671,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="58"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1683,15 +1683,15 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="62" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1704,7 +1704,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1727,7 +1727,7 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
@@ -1738,7 +1738,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="60"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="61"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
@@ -1780,7 +1780,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1809,7 +1809,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="65" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1823,7 +1823,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="63"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1835,7 +1835,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="63"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
@@ -1846,7 +1846,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="63"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1857,7 +1857,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="63"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="63"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1880,7 +1880,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="63"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="63"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="17" t="s">
         <v>14</v>
       </c>
@@ -1902,7 +1902,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="63"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1913,7 +1913,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="63"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="63"/>
+      <c r="A12" s="66"/>
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -1935,7 +1935,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="64"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="17" t="s">
         <v>16</v>
       </c>
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="68" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2023,7 +2023,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="66"/>
+      <c r="A3" s="69"/>
       <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="66"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="25" t="s">
         <v>38</v>
       </c>
@@ -2047,7 +2047,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="17" t="s">
         <v>39</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="67"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="17" t="s">
         <v>40</v>
       </c>
@@ -2071,11 +2071,11 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -2093,11 +2093,11 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="43"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="44"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2115,11 +2115,11 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2131,20 +2131,20 @@
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="34" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="45"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="44"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="71" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -2157,7 +2157,7 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="69"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="17" t="s">
         <v>47</v>
       </c>
@@ -2168,7 +2168,7 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="69"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
@@ -2179,7 +2179,7 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="70"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="17" t="s">
         <v>49</v>
       </c>
@@ -2190,11 +2190,11 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="46"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="44"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
@@ -2244,10 +2244,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79544C66-D72C-4E56-AF4D-5568E5F5A64B}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2275,293 +2275,293 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="54" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="60"/>
-      <c r="B3" s="50" t="s">
+      <c r="A3" s="63"/>
+      <c r="B3" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="54" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="60"/>
-      <c r="B4" s="50" t="s">
+      <c r="A4" s="63"/>
+      <c r="B4" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="54" t="s">
+      <c r="C4" s="48"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="60"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="54" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="60"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="54" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="60"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="54" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="60"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="63"/>
+      <c r="B8" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="54" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="54" t="s">
+      <c r="C9" s="48"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="60"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="54" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="54" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="54" t="s">
+      <c r="C12" s="48"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="54" t="s">
+      <c r="C13" s="48"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="60"/>
-      <c r="B14" s="50" t="s">
+      <c r="A14" s="63"/>
+      <c r="B14" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="54" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="60"/>
-      <c r="B15" s="50" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="54" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="60"/>
-      <c r="B16" s="53" t="s">
+      <c r="A16" s="63"/>
+      <c r="B16" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="54" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="60"/>
-      <c r="B17" s="50" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="54" t="s">
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="60"/>
-      <c r="B18" s="53" t="s">
+      <c r="A18" s="63"/>
+      <c r="B18" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="54" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="60"/>
-      <c r="B19" s="50" t="s">
+      <c r="A19" s="63"/>
+      <c r="B19" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="54" t="s">
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="60"/>
-      <c r="B20" s="50" t="s">
+      <c r="A20" s="63"/>
+      <c r="B20" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="54" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
-      <c r="B21" s="50" t="s">
+      <c r="A21" s="63"/>
+      <c r="B21" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="54" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="60"/>
-      <c r="B22" s="50" t="s">
+      <c r="A22" s="63"/>
+      <c r="B22" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="54" t="s">
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="60"/>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="63"/>
+      <c r="B23" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="54" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="50" t="s">
+      <c r="A24" s="64"/>
+      <c r="B24" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="54" t="s">
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="33"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="76" t="s">
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2574,7 +2574,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="72"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
@@ -2586,7 +2586,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="72"/>
+      <c r="A28" s="63"/>
       <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
@@ -2598,7 +2598,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="72"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="2" t="s">
         <v>59</v>
       </c>
@@ -2610,7 +2610,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="72"/>
+      <c r="A30" s="63"/>
       <c r="B30" s="2" t="s">
         <v>68</v>
       </c>
@@ -2622,7 +2622,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="72"/>
+      <c r="A31" s="63"/>
       <c r="B31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2634,7 +2634,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="72"/>
+      <c r="A32" s="63"/>
       <c r="B32" s="2" t="s">
         <v>54</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="72"/>
+      <c r="A33" s="63"/>
       <c r="B33" s="2" t="s">
         <v>55</v>
       </c>
@@ -2658,7 +2658,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="72"/>
+      <c r="A34" s="63"/>
       <c r="B34" s="29" t="s">
         <v>56</v>
       </c>
@@ -2670,7 +2670,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="72"/>
+      <c r="A35" s="63"/>
       <c r="B35" s="2" t="s">
         <v>57</v>
       </c>
@@ -2682,7 +2682,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="73"/>
+      <c r="A36" s="63"/>
       <c r="B36" s="2" t="s">
         <v>58</v>
       </c>
@@ -2694,30 +2694,31 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="34"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="33"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="68" t="s">
+      <c r="A38" s="81"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B39" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="69"/>
-      <c r="B39" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="C39" s="28" t="s">
         <v>18</v>
@@ -2726,76 +2727,80 @@
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="69"/>
+      <c r="A40" s="60"/>
       <c r="B40" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="4"/>
-      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="70"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="4"/>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="35"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="33"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="71" t="s">
+      <c r="A43" s="78"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="32"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="72"/>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="28"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="63"/>
+      <c r="B45" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="74"/>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="79"/>
+      <c r="B46" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="55" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="52" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
@@ -2804,12 +2809,19 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A44:A46"/>
     <mergeCell ref="A2:A24"/>
+    <mergeCell ref="A26:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2820,7 +2832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77982FF-C4D2-41E8-A83F-1D743BC8CBAF}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -2848,27 +2860,27 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="74" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="78" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="56"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="81"/>
+      <c r="A3" s="75"/>
       <c r="B3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="37"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -2879,120 +2891,120 @@
       <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="58" t="s">
         <v>95</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="37"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="37"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="37"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="37"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="37"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="37"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="37"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="37"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="37"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="37"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="37"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="37"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="37"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="37"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="37"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="55"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="52"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
@@ -3020,19 +3032,19 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="55" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour des sprints
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Sprint.xlsx
+++ b/Documents/Scrum/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF27F4B3-AECD-4459-8802-F8E600BD090E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C17340-1E58-4296-8125-87175679262A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_0." sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="197">
   <si>
     <t>STORY</t>
   </si>
@@ -77,10 +77,6 @@
 (modélisaton)</t>
   </si>
   <si>
-    <t>Créer le processus de l'application 
-(UseCase)</t>
-  </si>
-  <si>
     <t>Décrire les fonctionnalités de l'application</t>
   </si>
   <si>
@@ -92,15 +88,7 @@
 la création de l'application</t>
   </si>
   <si>
-    <t xml:space="preserve">Exprimer le problème existant au sein
- de l'entreprise </t>
-  </si>
-  <si>
     <t xml:space="preserve">Expliquer la méthodolgie (Scrum) pourquoi ce choix et quels sont les avantages </t>
-  </si>
-  <si>
-    <t>Expliquer les exigences que l'entreprises
-a du produit</t>
   </si>
   <si>
     <t>X</t>
@@ -162,33 +150,9 @@
     <t>Document plan d'assurance qualité</t>
   </si>
   <si>
-    <t>Définir commennt on travaille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Écrire ce que l'on va faire </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Décrire qui assure la communication 
-entre le groupe d'encadrment et le mandant </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Répondre à la question 
-de quoi faire </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Répondre à la question 
-de comment le faire </t>
-  </si>
-  <si>
     <t>Modélisation de la base de donnée</t>
   </si>
   <si>
-    <t>Créer la modélisation de la base de donnée</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Création d'accès pour les différents utilisateur</t>
   </si>
   <si>
@@ -207,13 +171,6 @@
     <t>Recherche sur l'API Google Map, agenda</t>
   </si>
   <si>
-    <t xml:space="preserve">Document de vision </t>
-  </si>
-  <si>
-    <t>Mettre à jour le document de vision après
-retour du groupe d'encadrement</t>
-  </si>
-  <si>
     <t>Maquette (sur Visual Studio)</t>
   </si>
   <si>
@@ -491,12 +448,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Maquette sur Visual Studio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création du login </t>
-  </si>
-  <si>
     <t>Créer le test LoginGood()</t>
   </si>
   <si>
@@ -586,9 +537,6 @@
   </si>
   <si>
     <t xml:space="preserve">Demander les identifianst à Waview  </t>
-  </si>
-  <si>
-    <t>Se connecte et aller sur le serveur + Php my admin</t>
   </si>
   <si>
     <t>Créer la classe Correspond</t>
@@ -628,18 +576,7 @@
     <t>API</t>
   </si>
   <si>
-    <t>Lier les différentes fenêtres 
-entre elles</t>
-  </si>
-  <si>
     <t>Base de données</t>
-  </si>
-  <si>
-    <t>Insérer dans table réservation
-ajouter id matériel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création fonction CRUD sur les tables </t>
   </si>
   <si>
     <t xml:space="preserve">Création filtre des headers </t>
@@ -679,11 +616,6 @@
 la base de données</t>
   </si>
   <si>
-    <t xml:space="preserve">Vérification des documents 
-(voir si ont les mets tous dans un 
-documents ou si on les sépare ) </t>
-  </si>
-  <si>
     <t>Finbalisation le designe</t>
   </si>
   <si>
@@ -721,20 +653,978 @@
     <t xml:space="preserve">Insérer la map à droite de la page </t>
   </si>
   <si>
-    <t xml:space="preserve">SE BASER SUR LES TABLES EN MAJUSCULES </t>
-  </si>
-  <si>
-    <t>/!\ ATTENTION mettre tous les crud pour toutes les tables comme sprint 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manuel utilisation </t>
+    <t>Finaliser la fenêtre "Chat"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauvegarder les activités </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauvegarder le chat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page hisorique des modifications </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page introduction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page pour les documents appliocables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page pour les documents références </t>
+  </si>
+  <si>
+    <t>Créer une page responsabilité associée au PAQ
+(avec chef de projet, responsable communication/documentation, reponsable qualité et responsable technique)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page pour les terminologies 
+(avec les termes utilisés et la signification des abreviations) </t>
+  </si>
+  <si>
+    <t>Créer une page pour la structure du projet 
+(avec l'équipe de projet et le comité de piolotage)</t>
+  </si>
+  <si>
+    <t>Créer une page pour les déamrche de développement
+(avec le cycle de développement, la description des phases et les actions à effectuer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page avec les documents por lagestion de projet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page pour les document techniques de réalisation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Décrire qui assure la communication entre le groupe d'encadrement et le mandant </t>
+  </si>
+  <si>
+    <t>Créer une page pour la structure de configuration 
+(avec l'identification documents/dossiers, état des documents et les différents répertoires)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page pour la gestion des modifications 
+(avec constat d'anomalie et demande d'évolution) </t>
+  </si>
+  <si>
+    <t>Créer une page explicant la livraison et installation du produit final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page explicative pour la reproduction et protection </t>
+  </si>
+  <si>
+    <t>Créer une page concernant les méthodes, outils et régles utilisés tout au long du projet)</t>
+  </si>
+  <si>
+    <t>Créer une page commentant les différents test de notre projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page conclusion résumant le document plan d'assurance qualité  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une page avec le but de l'application </t>
+  </si>
+  <si>
+    <t>Créer une page pour les logiciels concernés par le PAQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la fenêtre login </t>
+  </si>
+  <si>
+    <t>Lier les différentes fenêtres entre elles</t>
+  </si>
+  <si>
+    <t>Insérer dans table réservation ajouter id matériel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuel utilisateur </t>
+  </si>
+  <si>
+    <t>Manuel d'installation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavContact :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Créer la classe DATE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la classe PROJET</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavContact :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Créer la classe PHOTOGRAPHE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la classe EVENEMENT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavContact :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Créer la classe COLLABORATEUR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact :  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Créer la classe CLIENT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la classe PERSONNE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavCom : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Créer la classe DOCUMENT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavCom :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la classe MESSAGE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavCom : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Créer la classe CONTRAT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavCom : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Créer la classe DEVIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavCom :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la classe FACTURE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavMap : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la classe LIEU</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavMap :  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Créer la classe FICHIER_VIDEO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavMap :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Créer la classe PHOTO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavMap : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Créer la classe CRITERE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavContact :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Création fonction CRUD sur la table DATE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table PROJET</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavContact :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Création fonction CRUD sur la table PHOTOGRAPHE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table EVENEMENT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table COLLABORATEUR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table CLIENT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavContact : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table PERSONNE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavCom :  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table DOCUMENT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavCom : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table MESSAGE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WavCom : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table CONTRAT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavCom :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table DEVIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavCom :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Création fonction CRUD sur la table FACTURE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavMap :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table CRITERE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavMap :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Création fonction CRUD sur la table LIEU</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavMap :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table FICHIER_VIDEO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WavMap:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Création fonction CRUD sur la table PHOTO</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Vérification des documents (voir si ont les mets tous dans un 
+documents ou si on les sépare ) </t>
+  </si>
+  <si>
+    <t>Se connecter et aller sur le serveur + Php my admin</t>
+  </si>
+  <si>
+    <t>Créer la table Personne</t>
+  </si>
+  <si>
+    <t>Créer la table Document</t>
+  </si>
+  <si>
+    <t>Créer la table Projet</t>
+  </si>
+  <si>
+    <t>Créer la table Photo</t>
+  </si>
+  <si>
+    <t>Créer la table Critère</t>
+  </si>
+  <si>
+    <t>Créer la table FichierVidéo</t>
+  </si>
+  <si>
+    <t>Créer la table Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maquette modélisation base de données </t>
+  </si>
+  <si>
+    <t>Créer la modélisation de la base de donnée sur papier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la table Gere
+Lié à la table "Collaborateur" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la table Collaborateur 
+Lié à la table "Personne" </t>
+  </si>
+  <si>
+    <t>Créer la table Photographe
+Lié à la table "Personne"</t>
+  </si>
+  <si>
+    <t>Créer la table Client
+ Lié aux table "Personne" et "Projet"</t>
+  </si>
+  <si>
+    <t>Créer la table Evenement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la table Facture 
+Lié à la table "Document" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la table Devis 
+Lié à la table "Document" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la table Contrat
+Lié à la table "Document"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la table Concerne 
+Lié aux tables "Projet" et "Lieu" </t>
+  </si>
+  <si>
+    <t>Créer la table Lieu
+Lié aux tables "Photo" et "FichierVideo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer la table Correspond
+Lié aux tables "Lieu" et "Critere" </t>
+  </si>
+  <si>
+    <t>Créer la table A_Lieu
+Lié aux tables "Projet" et "Date"</t>
+  </si>
+  <si>
+    <t>Créer le table Consulte
+Lié aux tables "Lieu" et "Photographe"</t>
+  </si>
+  <si>
+    <t>Créer la table Contient
+Lié aux tables "Projet" et "Evenement"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exprimer le problème existant au sein de l'entreprise </t>
+  </si>
+  <si>
+    <t>Créer le processus de l'application (UseCase)</t>
+  </si>
+  <si>
+    <t>Expliquer les exigences que l'entreprises a du produit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,6 +1668,28 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -834,12 +1746,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -847,6 +1753,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8AEED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1153,7 +2065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1214,15 +2126,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1253,20 +2156,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1281,13 +2170,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1332,24 +2221,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1365,7 +2236,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1373,10 +2243,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1390,20 +2260,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1413,6 +2318,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FF9966FF"/>
+      <color rgb="FFEFC6FE"/>
       <color rgb="FFF8AEED"/>
       <color rgb="FFF583E5"/>
     </mruColors>
@@ -1727,8 +2635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3F248E-F3B8-4FD5-B554-6BF12D242858}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1755,178 +2663,178 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
-        <v>27</v>
+      <c r="A2" s="52" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="62"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="62"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="62"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="62"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="63"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="46"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="93"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="64" t="s">
-        <v>34</v>
+      <c r="A10" s="55" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="65"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="65"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="65"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="65"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="65"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="66"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1950,14 +2858,14 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1979,7 +2887,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="58" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1988,131 +2896,131 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="68"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="68"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="68"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="68"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="68"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="17" t="s">
-        <v>17</v>
+        <v>196</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="68"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="68"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="68"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
-        <v>11</v>
+        <v>195</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="68"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
-        <v>15</v>
+        <v>194</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="69"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
       <c r="B13" s="17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2148,16 +3056,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B15C13B-4F2C-4FF3-B337-5CE0DE76848B}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7265625" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2178,233 +3086,592 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="28"/>
+    <row r="2" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="25"/>
       <c r="D2" s="2"/>
       <c r="E2" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="71"/>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="28"/>
+    <row r="3" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="89"/>
+      <c r="B3" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="25"/>
       <c r="D3" s="2"/>
       <c r="E3" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="71"/>
-      <c r="B4" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="28"/>
+    <row r="4" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="89"/>
+      <c r="B4" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="25"/>
       <c r="D4" s="2"/>
       <c r="E4" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="71"/>
-      <c r="B5" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="28"/>
+    <row r="5" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="89"/>
+      <c r="B5" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="25"/>
       <c r="D5" s="2"/>
       <c r="E5" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="72"/>
-      <c r="B6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="28"/>
+    <row r="6" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="89"/>
+      <c r="B6" s="84" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="25"/>
       <c r="D6" s="2"/>
       <c r="E6" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="39"/>
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="89"/>
+      <c r="B7" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>18</v>
-      </c>
+    <row r="8" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="89"/>
+      <c r="B8" s="84" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="25"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="41"/>
+    <row r="9" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="89"/>
+      <c r="B9" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="28"/>
+    <row r="10" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="89"/>
+      <c r="B10" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="25"/>
       <c r="D10" s="2"/>
       <c r="E10" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="89"/>
+      <c r="B11" s="84" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="28"/>
+    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="89"/>
+      <c r="B12" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="25"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="34" t="s">
-        <v>18</v>
+      <c r="E12" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="41"/>
-    </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>18</v>
-      </c>
+    <row r="13" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="89"/>
+      <c r="B13" s="84" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="89"/>
+      <c r="B14" s="84" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="25"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="74"/>
-      <c r="B15" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>18</v>
-      </c>
+      <c r="E14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="89"/>
+      <c r="B15" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="25"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="74"/>
-      <c r="B16" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>18</v>
-      </c>
+      <c r="E15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="89"/>
+      <c r="B16" s="84" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="25"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="75"/>
-      <c r="B17" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>18</v>
-      </c>
+      <c r="E16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="89"/>
+      <c r="B17" s="84" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="25"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="43"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="41"/>
-    </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="28"/>
+      <c r="E17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="89"/>
+      <c r="B18" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="89"/>
+      <c r="B19" s="84" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="25"/>
       <c r="D19" s="2"/>
       <c r="E19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="89"/>
+      <c r="B20" s="84" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="90"/>
+      <c r="B21" s="84" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="85" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="56"/>
+      <c r="B26" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="56"/>
+      <c r="B27" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="56"/>
+      <c r="B28" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="56"/>
+      <c r="B29" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="56"/>
+      <c r="B30" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="56"/>
+      <c r="B31" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="56"/>
+      <c r="B32" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="56"/>
+      <c r="B33" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="56"/>
+      <c r="B34" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="56"/>
+      <c r="B35" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="56"/>
+      <c r="B36" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="56"/>
+      <c r="B37" s="87" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="25"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="56"/>
+      <c r="B38" s="86" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="56"/>
+      <c r="B39" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="56"/>
+      <c r="B40" s="86" t="s">
+        <v>190</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="56"/>
+      <c r="B41" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="56"/>
+      <c r="B42" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="56"/>
+      <c r="B43" s="86" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="56"/>
+      <c r="B44" s="86" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44" s="25"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="57"/>
+      <c r="B45" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="25"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="57"/>
+      <c r="B48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="25"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="5"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A14:A17"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A25:A45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2416,8 +3683,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:E42"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2445,531 +3712,531 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="51" t="s">
-        <v>18</v>
+      <c r="A2" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="42" t="s">
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="65"/>
-      <c r="B3" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="51" t="s">
-        <v>18</v>
+      <c r="A3" s="56"/>
+      <c r="B3" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42" t="s">
+        <v>15</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="65"/>
-      <c r="B4" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="51" t="s">
-        <v>18</v>
+      <c r="A4" s="56"/>
+      <c r="B4" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42" t="s">
+        <v>15</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="65"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="56"/>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="56"/>
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="56"/>
+      <c r="B8" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="56"/>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="56"/>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="56"/>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="56"/>
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="56"/>
+      <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="56"/>
+      <c r="B14" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="56"/>
+      <c r="B15" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="56"/>
+      <c r="B16" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="56"/>
+      <c r="B17" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="56"/>
+      <c r="B18" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="65"/>
-      <c r="B6" s="2" t="s">
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="56"/>
+      <c r="B19" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="65"/>
-      <c r="B7" s="2" t="s">
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="56"/>
+      <c r="B20" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="65"/>
-      <c r="B8" s="47" t="s">
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="56"/>
+      <c r="B21" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="65"/>
-      <c r="B9" s="2" t="s">
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="56"/>
+      <c r="B22" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="65"/>
-      <c r="B10" s="2" t="s">
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="56"/>
+      <c r="B23" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="65"/>
-      <c r="B11" s="2" t="s">
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="57"/>
+      <c r="B24" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="65"/>
-      <c r="B12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="65"/>
-      <c r="B13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="65"/>
-      <c r="B14" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="65"/>
-      <c r="B15" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="65"/>
-      <c r="B16" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="65"/>
-      <c r="B17" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="65"/>
-      <c r="B18" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="65"/>
-      <c r="B19" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="65"/>
-      <c r="B20" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="65"/>
-      <c r="B21" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="65"/>
-      <c r="B22" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="65"/>
-      <c r="B23" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="66"/>
-      <c r="B24" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="51" t="s">
-        <v>18</v>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="42" t="s">
+        <v>15</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="59"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="32"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="77" t="s">
-        <v>52</v>
+      <c r="A26" s="62" t="s">
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="65"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="65"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="65"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="65"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="65"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="65"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="65"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="65"/>
-      <c r="B34" s="29" t="s">
-        <v>56</v>
+      <c r="A34" s="56"/>
+      <c r="B34" s="26" t="s">
+        <v>44</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="65"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="65"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="65"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="60"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="32"/>
+      <c r="A38" s="51"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="76" t="s">
-        <v>45</v>
+      <c r="A39" s="61" t="s">
+        <v>35</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="62"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="28"/>
+        <v>37</v>
+      </c>
+      <c r="C40" s="25"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="34" t="s">
-        <v>18</v>
+      <c r="E40" s="31" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="62"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="4"/>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="63"/>
+      <c r="A42" s="54"/>
       <c r="B42" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="58"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="32"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="29"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="77" t="s">
-        <v>19</v>
+      <c r="A44" s="62" t="s">
+        <v>16</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="28"/>
+        <v>51</v>
+      </c>
+      <c r="C44" s="25"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="34" t="s">
-        <v>18</v>
+      <c r="E44" s="31" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="65"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="34" t="s">
-        <v>18</v>
+      <c r="E45" s="31" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="78"/>
+      <c r="A46" s="63"/>
       <c r="B46" s="6" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="52" t="s">
-        <v>18</v>
+      <c r="E46" s="43" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -3000,19 +4267,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77982FF-C4D2-41E8-A83F-1D743BC8CBAF}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -3029,388 +4296,800 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="79" t="s">
-        <v>45</v>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="64" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="80"/>
+      <c r="E2" s="31"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="65"/>
       <c r="B3" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="80"/>
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="65"/>
       <c r="B4" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="85"/>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="69"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="65"/>
+      <c r="B7" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="67"/>
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="65"/>
+      <c r="B8" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="67"/>
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="65"/>
+      <c r="B9" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="67"/>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="65"/>
+      <c r="B10" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="67"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="65"/>
+      <c r="B11" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="67"/>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="65"/>
+      <c r="B12" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="67"/>
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="79"/>
+      <c r="B13" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="67"/>
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="70"/>
+    </row>
+    <row r="15" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="81"/>
+      <c r="B16" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="47"/>
+      <c r="E16" s="31"/>
+    </row>
+    <row r="17" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="81"/>
+      <c r="B17" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="47"/>
+      <c r="E17" s="31"/>
+    </row>
+    <row r="18" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="81"/>
+      <c r="B18" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="31"/>
+    </row>
+    <row r="19" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="81"/>
+      <c r="B19" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="47"/>
+      <c r="E19" s="31"/>
+    </row>
+    <row r="20" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="81"/>
+      <c r="B20" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="47"/>
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="81"/>
+      <c r="B21" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="47"/>
+      <c r="E21" s="31"/>
+    </row>
+    <row r="22" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="81"/>
+      <c r="B22" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="47"/>
+      <c r="E22" s="31"/>
+    </row>
+    <row r="23" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="81"/>
+      <c r="B23" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="31"/>
+    </row>
+    <row r="24" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="81"/>
+      <c r="B24" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="47"/>
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="81"/>
+      <c r="B25" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="47"/>
+      <c r="E25" s="31"/>
+    </row>
+    <row r="26" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="81"/>
+      <c r="B26" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="47"/>
+      <c r="E26" s="31"/>
+    </row>
+    <row r="27" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="81"/>
+      <c r="B27" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="47"/>
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="81"/>
+      <c r="B28" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="47"/>
+      <c r="E28" s="31"/>
+    </row>
+    <row r="29" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="81"/>
+      <c r="B29" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="31"/>
+    </row>
+    <row r="30" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="81"/>
+      <c r="B30" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="47"/>
+      <c r="E30" s="31"/>
+    </row>
+    <row r="31" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="81"/>
+      <c r="B31" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="47"/>
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="81"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="31"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="81"/>
+      <c r="B33" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="47"/>
+      <c r="E33" s="31"/>
+      <c r="G33" s="78"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="81"/>
+      <c r="B34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="47"/>
+      <c r="E34" s="31"/>
+      <c r="G34" s="78"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="81"/>
+      <c r="B35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="47"/>
+      <c r="E35" s="31"/>
+      <c r="G35" s="78"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="81"/>
+      <c r="B36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="47"/>
+      <c r="E36" s="31"/>
+      <c r="G36" s="78"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="81"/>
+      <c r="B37" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="47"/>
+      <c r="E37" s="31"/>
+      <c r="G37" s="78"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="81"/>
+      <c r="B38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="47"/>
+      <c r="E38" s="31"/>
+      <c r="G38" s="78"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="81"/>
+      <c r="B39" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="47"/>
+      <c r="E39" s="31"/>
+      <c r="G39" s="78"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="81"/>
+      <c r="B40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="47"/>
+      <c r="E40" s="31"/>
+      <c r="G40" s="78"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="81"/>
+      <c r="B41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="31"/>
+      <c r="G41" s="78"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="81"/>
+      <c r="B42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="47"/>
+      <c r="E42" s="31"/>
+      <c r="G42" s="78"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="81"/>
+      <c r="B43" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="47"/>
+      <c r="E43" s="31"/>
+      <c r="G43" s="78"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="81"/>
+      <c r="B44" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="47"/>
+      <c r="E44" s="31"/>
+      <c r="G44" s="78"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="81"/>
+      <c r="B45" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="47"/>
+      <c r="E45" s="31"/>
+      <c r="G45" s="78"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="81"/>
+      <c r="B46" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="47"/>
+      <c r="E46" s="31"/>
+      <c r="G46" s="78"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="81"/>
+      <c r="B47" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="47"/>
+      <c r="E47" s="31"/>
+      <c r="G47" s="78"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="81"/>
+      <c r="B48" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C48" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="47"/>
+      <c r="E48" s="31"/>
+      <c r="G48" s="78"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="69"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="70"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="47"/>
+      <c r="E50" s="31"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="81"/>
+      <c r="B51" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="47"/>
+      <c r="E51" s="31"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="82"/>
+      <c r="B52" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="47"/>
+      <c r="E52" s="31"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="69"/>
+      <c r="B53" s="69"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="47"/>
+      <c r="E54" s="31"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="65"/>
+      <c r="B55" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="47"/>
+      <c r="E55" s="31"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="65"/>
+      <c r="B56" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="47"/>
+      <c r="E56" s="31"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="65"/>
+      <c r="B57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="47"/>
+      <c r="E57" s="31"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="65"/>
+      <c r="B58" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="47"/>
+      <c r="E58" s="31"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="65"/>
+      <c r="B59" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="73"/>
+      <c r="E59" s="74"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="65"/>
+      <c r="B60" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="73"/>
+      <c r="E60" s="74"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="65"/>
+      <c r="B61" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="73"/>
+      <c r="E61" s="74"/>
+    </row>
+    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="65"/>
+      <c r="B62" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="81"/>
-      <c r="B7" s="82" t="s">
+      <c r="C62" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="73"/>
+      <c r="E62" s="74"/>
+    </row>
+    <row r="63" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" s="79"/>
+      <c r="B63" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="73"/>
+      <c r="E63" s="74"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="69"/>
+      <c r="B64" s="69"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="69"/>
+      <c r="E64" s="77"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="73"/>
+      <c r="E65" s="74"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="65"/>
+      <c r="B66" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="73"/>
+      <c r="E66" s="74"/>
+    </row>
+    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="65"/>
+      <c r="B67" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="81"/>
-      <c r="B8" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="81"/>
-      <c r="B9" s="93" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="34"/>
-    </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="81"/>
-      <c r="B10" s="84" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="34"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="85"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="86"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="34"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="34"/>
-      <c r="G13" s="96" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="92"/>
-      <c r="B14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="34"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="34"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="85"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="86"/>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="34"/>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="92"/>
-      <c r="B18" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="34"/>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="92"/>
-      <c r="B19" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="34"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="85"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="C67" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="73"/>
+      <c r="E67" s="74"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="65"/>
+      <c r="B68" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="C68" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="73"/>
+      <c r="E68" s="74"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="65"/>
+      <c r="B69" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C69" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="73"/>
+      <c r="E69" s="74"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="65"/>
+      <c r="B70" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="34"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2" t="s">
+      <c r="C70" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="73"/>
+      <c r="E70" s="74"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="79"/>
+      <c r="B71" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="34"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="34"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="34"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="34"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="87"/>
-      <c r="B26" s="88" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="90"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="87"/>
-      <c r="B27" s="88" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="90"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="87"/>
-      <c r="B28" s="88" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="90"/>
-    </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="87"/>
-      <c r="B29" s="91" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="90"/>
-    </row>
-    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="87"/>
-      <c r="B30" s="91" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="90"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="85"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="94"/>
-    </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="87" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" s="91" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="90"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="87"/>
-      <c r="B33" s="91" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="90"/>
-    </row>
-    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="87"/>
-      <c r="B34" s="91" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="90"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="87"/>
-      <c r="B35" s="91" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="90"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="87"/>
-      <c r="B36" s="91" t="s">
-        <v>123</v>
-      </c>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="90"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="87"/>
-      <c r="B37" s="91" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="90"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="87"/>
-      <c r="B38" s="91" t="s">
-        <v>125</v>
-      </c>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="90"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="97"/>
-      <c r="B39" s="95"/>
-      <c r="C39" s="98"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="94"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="87" t="s">
-        <v>129</v>
-      </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="89"/>
-      <c r="D40" s="89"/>
-      <c r="E40" s="90"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="87"/>
-      <c r="B41" s="91"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="90"/>
-    </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="52"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="C71" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="73"/>
+      <c r="E71" s="74"/>
+    </row>
+    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="5"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="43"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="A65:A71"/>
     <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A15:A48"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A54:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3421,31 +5100,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF97C5A-E76A-4F7F-AE1B-EEE4815545E3}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="46" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
+      <c r="A2" s="71" t="s">
+        <v>134</v>
+      </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -3453,7 +5137,9 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>

</xml_diff>